<commit_message>
added stir calcs and crop type
</commit_message>
<xml_diff>
--- a/data/tillage records.xlsx
+++ b/data/tillage records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7d62234183fd3ba/Documents/GitHub/kerbel-long-term-impacts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="238" documentId="11_F25DC773A252ABDACC10484E2159436A5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A35101C2-0CDB-4526-ADA5-6522C2902448}"/>
+  <xr:revisionPtr revIDLastSave="314" documentId="11_F25DC773A252ABDACC10484E2159436A5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBD6CE6B-980F-499D-96C4-7CDA6AA6E07F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="780" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -1308,9 +1308,6 @@
     <t>https://www.yetterco.com/products/11-plantermount-row-cleaners/310-2967-rigid-row-cleaner</t>
   </si>
   <si>
-    <t>Use (measured furrow width / row spacing)</t>
-  </si>
-  <si>
     <t>Use (measured ditch width / row spacing)</t>
   </si>
   <si>
@@ -1345,6 +1342,9 @@
   </si>
   <si>
     <t>Area Fraction = width of disturbed soil band/row spacing</t>
+  </si>
+  <si>
+    <t>0.13–0.21</t>
   </si>
 </sst>
 </file>
@@ -1429,6 +1429,9 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1464,9 +1467,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1481,7 +1481,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AF96C6C4-2044-4D28-897C-4304D857D445}" name="Table2" displayName="Table2" ref="A20:D94" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AF96C6C4-2044-4D28-897C-4304D857D445}" name="Table2" displayName="Table2" ref="A20:D94" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A20:D94" xr:uid="{AF96C6C4-2044-4D28-897C-4304D857D445}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{6BDD50D5-74D6-44DA-9B41-5758246A6955}" name="Implement"/>
@@ -1494,7 +1494,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BFBC9A84-6A61-49B2-A66D-5752FA5C08F5}" name="Table4" displayName="Table4" ref="H20:M54" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BFBC9A84-6A61-49B2-A66D-5752FA5C08F5}" name="Table4" displayName="Table4" ref="H20:M54" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="H20:M54" xr:uid="{BFBC9A84-6A61-49B2-A66D-5752FA5C08F5}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{316B493A-FB77-428B-A9AA-405EDFE2FC10}" name="My Operation"/>
@@ -1526,7 +1526,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{065CF52D-11DD-448D-BCEB-C76903A49E5F}" name="Table1" displayName="Table1" ref="A1:I259">
   <autoFilter ref="A1:I259" xr:uid="{065CF52D-11DD-448D-BCEB-C76903A49E5F}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C7DBE28E-9D69-4F94-83DC-894A2EF7042A}" name="Date" totalsRowLabel="Total" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C7DBE28E-9D69-4F94-83DC-894A2EF7042A}" name="Date" totalsRowLabel="Total" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A74729C6-F806-40A5-B341-BD394DA8F956}" name="CT Operation"/>
     <tableColumn id="3" xr3:uid="{A01DF9F1-9072-46F5-8641-4D1A13F146A2}" name="ST Operation"/>
     <tableColumn id="4" xr3:uid="{911A169D-B978-45C7-B117-7F2754D4B64B}" name="MT Operation"/>
@@ -1805,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4F6CE9-55F5-477C-9293-7F822A7FD663}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76:I82"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="J79" sqref="J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3043,7 +3043,7 @@
         <v>0.7</v>
       </c>
       <c r="H57" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3643,13 +3643,13 @@
         <v>18</v>
       </c>
       <c r="I78">
-        <v>0.3</v>
+        <v>0.17</v>
       </c>
       <c r="J78" t="s">
-        <v>397</v>
+        <v>435</v>
       </c>
       <c r="K78" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="L78" t="s">
         <v>398</v>
@@ -3678,7 +3678,7 @@
         <v>397</v>
       </c>
       <c r="K79" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L79" t="s">
         <v>398</v>
@@ -3707,7 +3707,7 @@
         <v>397</v>
       </c>
       <c r="K80" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L80" t="s">
         <v>398</v>
@@ -3736,7 +3736,7 @@
         <v>397</v>
       </c>
       <c r="K81" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L81" t="s">
         <v>398</v>
@@ -3765,7 +3765,7 @@
         <v>397</v>
       </c>
       <c r="K82" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L82" t="s">
         <v>398</v>
@@ -3794,7 +3794,7 @@
         <v>0</v>
       </c>
       <c r="K83" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L83" t="s">
         <v>353</v>
@@ -3823,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="K84" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L84" t="s">
         <v>353</v>
@@ -3852,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="K85" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L85" t="s">
         <v>353</v>
@@ -3881,7 +3881,7 @@
         <v>0</v>
       </c>
       <c r="K86" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L86" t="s">
         <v>353</v>
@@ -3910,7 +3910,7 @@
         <v>0</v>
       </c>
       <c r="K87" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L87" t="s">
         <v>353</v>
@@ -3939,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="K88" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L88" t="s">
         <v>353</v>
@@ -3968,7 +3968,7 @@
         <v>0</v>
       </c>
       <c r="K89" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L89" t="s">
         <v>353</v>
@@ -3988,7 +3988,7 @@
         <v>0.25</v>
       </c>
       <c r="H90" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I90">
         <v>0.27</v>
@@ -3997,7 +3997,7 @@
         <v>393</v>
       </c>
       <c r="K90" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L90" t="s">
         <v>406</v>
@@ -4046,7 +4046,7 @@
         <v>0.25</v>
       </c>
       <c r="H92" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I92">
         <v>0</v>
@@ -4055,7 +4055,7 @@
         <v>0</v>
       </c>
       <c r="K92" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L92" t="s">
         <v>353</v>
@@ -4232,7 +4232,7 @@
         <v>0</v>
       </c>
       <c r="K101" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L101" t="s">
         <v>353</v>
@@ -4249,7 +4249,7 @@
         <v>0</v>
       </c>
       <c r="K102" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L102" t="s">
         <v>353</v>
@@ -4266,7 +4266,7 @@
         <v>0</v>
       </c>
       <c r="K103" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L103" t="s">
         <v>353</v>
@@ -4283,7 +4283,7 @@
         <v>0</v>
       </c>
       <c r="K104" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L104" t="s">
         <v>353</v>
@@ -4300,7 +4300,7 @@
         <v>0</v>
       </c>
       <c r="K105" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L105" t="s">
         <v>353</v>
@@ -4317,7 +4317,7 @@
         <v>0</v>
       </c>
       <c r="K106" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L106" t="s">
         <v>353</v>
@@ -4334,7 +4334,7 @@
         <v>0</v>
       </c>
       <c r="K107" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L107" t="s">
         <v>353</v>
@@ -4351,7 +4351,7 @@
         <v>0</v>
       </c>
       <c r="K108" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L108" t="s">
         <v>353</v>
@@ -4368,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="K109" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L109" t="s">
         <v>353</v>
@@ -4385,13 +4385,14 @@
         <v>0</v>
       </c>
       <c r="K110" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L110" t="s">
         <v>353</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A18" r:id="rId1" display="CULT Factors Table A-9 from SWAT TAMU User's Manual, Version 200, page 386" xr:uid="{B850B8E0-2318-4030-A997-9B050EA94117}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
fixed labeling and added debug code
</commit_message>
<xml_diff>
--- a/data/tillage records.xlsx
+++ b/data/tillage records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7d62234183fd3ba/Documents/GitHub/kerbel-long-term-impacts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="11_F25DC773A252ABDACC10484E2159436A5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D1E3634-3BBE-473B-B2D1-35B0FD3D68E8}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="11_F25DC773A252ABDACC10484E2159436A5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C9E0DCD-7E50-46AB-8983-2A656097A544}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="780" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tillage records" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="186">
   <si>
     <t>Date</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Bale Stalks</t>
-  </si>
-  <si>
-    <t>11/25/215</t>
   </si>
   <si>
     <t>Strip Till + Fertilizer Application*</t>
@@ -959,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B146" sqref="B144:B146"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,28 +976,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
         <v>173</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" t="s">
-        <v>175</v>
-      </c>
       <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" t="s">
-        <v>72</v>
-      </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1011,16 +1008,16 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2">
         <v>189</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1031,19 +1028,19 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3">
         <v>205</v>
       </c>
       <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
         <v>77</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>78</v>
-      </c>
-      <c r="I3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1054,13 +1051,13 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4">
         <v>205</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1071,19 +1068,19 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5">
         <v>180</v>
       </c>
       <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" t="s">
         <v>81</v>
-      </c>
-      <c r="H5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1094,16 +1091,16 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6">
         <v>180</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1114,16 +1111,16 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7">
         <v>189</v>
       </c>
       <c r="G7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" t="s">
         <v>83</v>
-      </c>
-      <c r="H7" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1134,16 +1131,16 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8">
         <v>189</v>
       </c>
       <c r="G8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" t="s">
         <v>83</v>
-      </c>
-      <c r="H8" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1154,16 +1151,16 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9">
         <v>156</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1174,13 +1171,13 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10">
         <v>156</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1197,16 +1194,16 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11">
         <v>130</v>
       </c>
       <c r="G11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1223,16 +1220,16 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12">
         <v>130</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1243,16 +1240,16 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13">
         <v>189</v>
       </c>
       <c r="G13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" t="s">
         <v>89</v>
-      </c>
-      <c r="I13" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1283,13 +1280,13 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F15">
         <v>144</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1306,16 +1303,16 @@
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F16">
         <v>156</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1332,7 +1329,7 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1349,7 +1346,7 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1366,7 +1363,7 @@
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1377,16 +1374,16 @@
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F20">
         <v>189</v>
       </c>
       <c r="G20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" t="s">
         <v>97</v>
-      </c>
-      <c r="H20" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1397,13 +1394,13 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F21">
         <v>205</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1414,16 +1411,16 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F22">
         <v>180</v>
       </c>
       <c r="G22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1434,16 +1431,16 @@
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23">
         <v>180</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1454,16 +1451,16 @@
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F24">
         <v>189</v>
       </c>
       <c r="G24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" t="s">
         <v>83</v>
-      </c>
-      <c r="H24" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1474,16 +1471,16 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F25">
         <v>189</v>
       </c>
       <c r="G25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" t="s">
         <v>83</v>
-      </c>
-      <c r="H25" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1494,13 +1491,13 @@
         <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F26">
         <v>189</v>
       </c>
       <c r="G26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1511,16 +1508,16 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F27">
         <v>189</v>
       </c>
       <c r="G27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1531,16 +1528,16 @@
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F28">
         <v>156</v>
       </c>
       <c r="G28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1551,16 +1548,16 @@
         <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F29">
         <v>189</v>
       </c>
       <c r="G29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1571,13 +1568,13 @@
         <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F30">
         <v>189</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1594,16 +1591,16 @@
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F31">
         <v>130</v>
       </c>
       <c r="G31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1620,13 +1617,13 @@
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F32">
         <v>144</v>
       </c>
       <c r="G32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1634,19 +1631,19 @@
         <v>41039</v>
       </c>
       <c r="B33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F33">
         <v>156</v>
       </c>
       <c r="G33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1668,22 +1665,22 @@
         <v>41064</v>
       </c>
       <c r="B35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F35">
         <v>156</v>
       </c>
       <c r="G35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1697,13 +1694,13 @@
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F36">
         <v>189</v>
       </c>
       <c r="G36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1734,13 +1731,13 @@
         <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F38">
         <v>144</v>
       </c>
       <c r="G38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1757,16 +1754,16 @@
         <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F39">
         <v>156</v>
       </c>
       <c r="G39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1783,7 +1780,7 @@
         <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1800,7 +1797,7 @@
         <v>14</v>
       </c>
       <c r="G41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1817,7 +1814,7 @@
         <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1828,13 +1825,13 @@
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F43">
         <v>205</v>
       </c>
       <c r="G43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1845,16 +1842,16 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F44">
         <v>189</v>
       </c>
       <c r="G44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1865,16 +1862,16 @@
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F45">
         <v>189</v>
       </c>
       <c r="G45" t="s">
+        <v>82</v>
+      </c>
+      <c r="H45" t="s">
         <v>83</v>
-      </c>
-      <c r="H45" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1891,16 +1888,16 @@
         <v>18</v>
       </c>
       <c r="E46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F46">
         <v>189</v>
       </c>
       <c r="G46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1917,13 +1914,13 @@
         <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F47">
         <v>156</v>
       </c>
       <c r="G47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1940,16 +1937,16 @@
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F48">
         <v>189</v>
       </c>
       <c r="G48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -1966,19 +1963,19 @@
         <v>19</v>
       </c>
       <c r="E49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F49">
         <v>189</v>
       </c>
       <c r="G49" t="s">
+        <v>100</v>
+      </c>
+      <c r="H49" t="s">
+        <v>74</v>
+      </c>
+      <c r="I49" t="s">
         <v>101</v>
-      </c>
-      <c r="H49" t="s">
-        <v>75</v>
-      </c>
-      <c r="I49" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2009,16 +2006,16 @@
         <v>20</v>
       </c>
       <c r="E51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F51">
         <v>189</v>
       </c>
       <c r="G51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2049,10 +2046,10 @@
         <v>21</v>
       </c>
       <c r="E53" t="s">
+        <v>102</v>
+      </c>
+      <c r="G53" t="s">
         <v>103</v>
-      </c>
-      <c r="G53" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2063,16 +2060,16 @@
         <v>22</v>
       </c>
       <c r="E54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F54">
         <v>189</v>
       </c>
       <c r="G54" t="s">
+        <v>96</v>
+      </c>
+      <c r="H54" t="s">
         <v>97</v>
-      </c>
-      <c r="H54" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2083,13 +2080,13 @@
         <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F55">
         <v>205</v>
       </c>
       <c r="G55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2100,16 +2097,16 @@
         <v>23</v>
       </c>
       <c r="E56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F56">
         <v>205</v>
       </c>
       <c r="G56" t="s">
+        <v>104</v>
+      </c>
+      <c r="H56" t="s">
         <v>105</v>
-      </c>
-      <c r="H56" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2120,16 +2117,16 @@
         <v>23</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F57">
         <v>156</v>
       </c>
       <c r="G57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2140,16 +2137,16 @@
         <v>5</v>
       </c>
       <c r="E58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F58">
         <v>205</v>
       </c>
       <c r="G58" t="s">
+        <v>82</v>
+      </c>
+      <c r="H58" t="s">
         <v>83</v>
-      </c>
-      <c r="H58" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2166,16 +2163,16 @@
         <v>24</v>
       </c>
       <c r="E59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F59">
         <v>205</v>
       </c>
       <c r="G59" t="s">
+        <v>76</v>
+      </c>
+      <c r="H59" t="s">
         <v>77</v>
-      </c>
-      <c r="H59" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2186,16 +2183,16 @@
         <v>23</v>
       </c>
       <c r="E60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F60">
         <v>205</v>
       </c>
       <c r="G60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2206,16 +2203,16 @@
         <v>25</v>
       </c>
       <c r="E61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F61">
         <v>189</v>
       </c>
       <c r="G61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2226,13 +2223,13 @@
         <v>23</v>
       </c>
       <c r="E62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F62">
         <v>144</v>
       </c>
       <c r="G62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2249,16 +2246,16 @@
         <v>26</v>
       </c>
       <c r="E63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F63">
         <v>189</v>
       </c>
       <c r="G63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2289,16 +2286,16 @@
         <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F65">
         <v>180</v>
       </c>
       <c r="G65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2315,10 +2312,10 @@
         <v>27</v>
       </c>
       <c r="E66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2335,7 +2332,7 @@
         <v>28</v>
       </c>
       <c r="G67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2352,7 +2349,7 @@
         <v>29</v>
       </c>
       <c r="G68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2363,16 +2360,16 @@
         <v>16</v>
       </c>
       <c r="E69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F69">
         <v>180</v>
       </c>
       <c r="G69" t="s">
+        <v>96</v>
+      </c>
+      <c r="H69" t="s">
         <v>97</v>
-      </c>
-      <c r="H69" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2391,13 +2388,13 @@
         <v>3</v>
       </c>
       <c r="E71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F71">
         <v>205</v>
       </c>
       <c r="G71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -2414,16 +2411,16 @@
         <v>23</v>
       </c>
       <c r="E72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F72">
         <v>144</v>
       </c>
       <c r="G72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -2437,16 +2434,16 @@
         <v>31</v>
       </c>
       <c r="E73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F73">
         <v>189</v>
       </c>
       <c r="G73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -2460,13 +2457,13 @@
         <v>33</v>
       </c>
       <c r="E74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F74">
         <v>189</v>
       </c>
       <c r="G74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -2477,16 +2474,16 @@
         <v>34</v>
       </c>
       <c r="E75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F75">
         <v>189</v>
       </c>
       <c r="G75" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -2497,16 +2494,16 @@
         <v>23</v>
       </c>
       <c r="E76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F76">
         <v>144</v>
       </c>
       <c r="G76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -2517,13 +2514,13 @@
         <v>9</v>
       </c>
       <c r="E77" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F77">
         <v>100</v>
       </c>
       <c r="G77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -2540,16 +2537,16 @@
         <v>26</v>
       </c>
       <c r="E78" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F78">
         <v>189</v>
       </c>
       <c r="G78" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -2566,16 +2563,16 @@
         <v>11</v>
       </c>
       <c r="E79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -2592,16 +2589,16 @@
         <v>12</v>
       </c>
       <c r="E80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F80">
         <v>156</v>
       </c>
       <c r="G80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H80" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -2615,16 +2612,16 @@
         <v>35</v>
       </c>
       <c r="E81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F81">
         <v>156</v>
       </c>
       <c r="G81" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -2641,7 +2638,7 @@
         <v>27</v>
       </c>
       <c r="E82" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -2658,7 +2655,7 @@
         <v>28</v>
       </c>
       <c r="G83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -2675,27 +2672,27 @@
         <v>36</v>
       </c>
       <c r="G84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>37</v>
+      <c r="A85" s="1">
+        <v>42333</v>
       </c>
       <c r="B85" t="s">
         <v>16</v>
       </c>
       <c r="E85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F85">
         <v>350</v>
       </c>
       <c r="G85" t="s">
+        <v>114</v>
+      </c>
+      <c r="I85" t="s">
         <v>115</v>
-      </c>
-      <c r="I85" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -2712,13 +2709,13 @@
         <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F86">
         <v>156</v>
       </c>
       <c r="G86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -2735,16 +2732,16 @@
         <v>30</v>
       </c>
       <c r="E87" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F87">
         <v>345</v>
       </c>
       <c r="G87" t="s">
+        <v>118</v>
+      </c>
+      <c r="I87" t="s">
         <v>119</v>
-      </c>
-      <c r="I87" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -2755,13 +2752,13 @@
         <v>30</v>
       </c>
       <c r="E88" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F88">
         <v>345</v>
       </c>
       <c r="G88" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -2772,13 +2769,13 @@
         <v>3</v>
       </c>
       <c r="E89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F89">
         <v>205</v>
       </c>
       <c r="G89" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -2789,16 +2786,16 @@
         <v>23</v>
       </c>
       <c r="E90" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F90">
         <v>205</v>
       </c>
       <c r="G90" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -2809,16 +2806,16 @@
         <v>5</v>
       </c>
       <c r="E91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F91">
         <v>205</v>
       </c>
       <c r="G91" t="s">
+        <v>82</v>
+      </c>
+      <c r="H91" t="s">
         <v>83</v>
-      </c>
-      <c r="H91" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -2829,22 +2826,22 @@
         <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D92" t="s">
         <v>9</v>
       </c>
       <c r="E92" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F92">
         <v>189</v>
       </c>
       <c r="G92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H92" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -2861,16 +2858,16 @@
         <v>18</v>
       </c>
       <c r="E93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F93">
         <v>189</v>
       </c>
       <c r="G93" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H93" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -2881,16 +2878,16 @@
         <v>23</v>
       </c>
       <c r="E94" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F94">
         <v>158</v>
       </c>
       <c r="G94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -2907,13 +2904,13 @@
         <v>7</v>
       </c>
       <c r="E95" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F95">
         <v>156</v>
       </c>
       <c r="G95" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -2921,19 +2918,19 @@
         <v>42432</v>
       </c>
       <c r="B96" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C96" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D96" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G96" t="s">
+        <v>121</v>
+      </c>
+      <c r="I96" t="s">
         <v>122</v>
-      </c>
-      <c r="I96" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -2955,16 +2952,16 @@
         <v>42576</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C98" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D98" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -2972,16 +2969,16 @@
         <v>42577</v>
       </c>
       <c r="B99" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C99" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D99" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G99" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3020,13 +3017,13 @@
         <v>3</v>
       </c>
       <c r="E102" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F102">
         <v>295</v>
       </c>
       <c r="G102" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3037,16 +3034,16 @@
         <v>23</v>
       </c>
       <c r="E103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F103">
         <v>189</v>
       </c>
       <c r="G103" t="s">
+        <v>104</v>
+      </c>
+      <c r="H103" t="s">
         <v>105</v>
-      </c>
-      <c r="H103" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -3057,16 +3054,16 @@
         <v>23</v>
       </c>
       <c r="E104" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F104">
         <v>156</v>
       </c>
       <c r="G104" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H104" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -3077,16 +3074,16 @@
         <v>5</v>
       </c>
       <c r="E105" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F105">
         <v>245</v>
       </c>
       <c r="G105" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H105" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -3094,19 +3091,19 @@
         <v>42835</v>
       </c>
       <c r="B106" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E106" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F106">
         <v>144</v>
       </c>
       <c r="G106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H106" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -3114,13 +3111,13 @@
         <v>42835</v>
       </c>
       <c r="C107" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D107" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G107" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -3128,22 +3125,22 @@
         <v>42838</v>
       </c>
       <c r="C108" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D108" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E108" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F108">
         <v>295</v>
       </c>
       <c r="G108" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H108" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -3160,16 +3157,16 @@
         <v>18</v>
       </c>
       <c r="E109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F109">
         <v>189</v>
       </c>
       <c r="G109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H109" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -3180,16 +3177,16 @@
         <v>23</v>
       </c>
       <c r="E110" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F110">
         <v>144</v>
       </c>
       <c r="G110" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H110" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -3200,13 +3197,13 @@
         <v>23</v>
       </c>
       <c r="E111" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F111">
         <v>144</v>
       </c>
       <c r="G111" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -3223,16 +3220,16 @@
         <v>19</v>
       </c>
       <c r="E112" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F112">
         <v>189</v>
       </c>
       <c r="G112" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H112" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -3240,22 +3237,22 @@
         <v>42907</v>
       </c>
       <c r="C113" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D113" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E113" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F113">
         <v>89</v>
       </c>
       <c r="G113" t="s">
+        <v>128</v>
+      </c>
+      <c r="H113" t="s">
         <v>129</v>
-      </c>
-      <c r="H113" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -3272,16 +3269,16 @@
         <v>12</v>
       </c>
       <c r="E114" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F114">
         <v>189</v>
       </c>
       <c r="G114" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H114" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -3298,10 +3295,10 @@
         <v>21</v>
       </c>
       <c r="E115" t="s">
+        <v>102</v>
+      </c>
+      <c r="G115" t="s">
         <v>103</v>
-      </c>
-      <c r="G115" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -3312,16 +3309,16 @@
         <v>30</v>
       </c>
       <c r="E116" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F116">
         <v>245</v>
       </c>
       <c r="G116" t="s">
+        <v>131</v>
+      </c>
+      <c r="H116" t="s">
         <v>132</v>
-      </c>
-      <c r="H116" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -3332,13 +3329,13 @@
         <v>3</v>
       </c>
       <c r="E117" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F117">
         <v>295</v>
       </c>
       <c r="G117" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -3349,16 +3346,16 @@
         <v>23</v>
       </c>
       <c r="E118" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F118">
         <v>130</v>
       </c>
       <c r="G118" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H118" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -3369,16 +3366,16 @@
         <v>23</v>
       </c>
       <c r="E119" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F119">
         <v>130</v>
       </c>
       <c r="G119" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H119" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -3389,16 +3386,16 @@
         <v>5</v>
       </c>
       <c r="E120" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F120">
         <v>295</v>
       </c>
       <c r="G120" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H120" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3409,16 +3406,16 @@
         <v>23</v>
       </c>
       <c r="E121" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F121">
         <v>130</v>
       </c>
       <c r="G121" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H121" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -3429,13 +3426,13 @@
         <v>9</v>
       </c>
       <c r="E122" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F122">
         <v>144</v>
       </c>
       <c r="G122" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -3452,16 +3449,16 @@
         <v>12</v>
       </c>
       <c r="E123" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F123">
         <v>295</v>
       </c>
       <c r="G123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H123" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -3478,16 +3475,16 @@
         <v>11</v>
       </c>
       <c r="E124" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F124" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G124" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H124" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -3495,22 +3492,22 @@
         <v>43237</v>
       </c>
       <c r="B125" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C125" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D125" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E125" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F125">
         <v>189</v>
       </c>
       <c r="G125" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -3518,22 +3515,22 @@
         <v>43238</v>
       </c>
       <c r="C126" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D126" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E126" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F126">
         <v>295</v>
       </c>
       <c r="G126" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H126" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -3544,16 +3541,16 @@
         <v>7</v>
       </c>
       <c r="D127" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E127" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F127">
         <v>130</v>
       </c>
       <c r="G127" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -3561,19 +3558,19 @@
         <v>43238</v>
       </c>
       <c r="B128" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C128" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D128" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G128" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H128" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -3590,16 +3587,16 @@
         <v>12</v>
       </c>
       <c r="E129" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F129">
         <v>130</v>
       </c>
       <c r="G129" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H129" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -3616,16 +3613,16 @@
         <v>35</v>
       </c>
       <c r="E130" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F130">
         <v>156</v>
       </c>
       <c r="G130" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H130" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -3642,16 +3639,16 @@
         <v>12</v>
       </c>
       <c r="E131" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F131">
         <v>130</v>
       </c>
       <c r="G131" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H131" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -3659,19 +3656,19 @@
         <v>43342</v>
       </c>
       <c r="B132" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C132" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D132" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E132" t="s">
+        <v>137</v>
+      </c>
+      <c r="I132" t="s">
         <v>138</v>
-      </c>
-      <c r="I132" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -3679,19 +3676,19 @@
         <v>43347</v>
       </c>
       <c r="B133" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C133" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D133" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E133" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G133" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -3708,16 +3705,16 @@
         <v>30</v>
       </c>
       <c r="E134" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F134">
         <v>380</v>
       </c>
       <c r="G134" t="s">
+        <v>141</v>
+      </c>
+      <c r="H134" t="s">
         <v>142</v>
-      </c>
-      <c r="H134" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -3734,16 +3731,16 @@
         <v>30</v>
       </c>
       <c r="E135" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F135">
         <v>380</v>
       </c>
       <c r="G135" t="s">
+        <v>141</v>
+      </c>
+      <c r="H135" t="s">
         <v>142</v>
-      </c>
-      <c r="H135" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -3751,13 +3748,13 @@
         <v>43353</v>
       </c>
       <c r="B136" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C136" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D136" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -3774,16 +3771,16 @@
         <v>23</v>
       </c>
       <c r="E137" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F137">
         <v>189</v>
       </c>
       <c r="G137" t="s">
+        <v>104</v>
+      </c>
+      <c r="H137" t="s">
         <v>105</v>
-      </c>
-      <c r="H137" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -3800,16 +3797,16 @@
         <v>18</v>
       </c>
       <c r="E138" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F138">
         <v>245</v>
       </c>
       <c r="G138" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H138" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -3826,13 +3823,13 @@
         <v>7</v>
       </c>
       <c r="E139" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F139">
         <v>156</v>
       </c>
       <c r="G139" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -3849,13 +3846,13 @@
         <v>9</v>
       </c>
       <c r="E140" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F140">
         <v>144</v>
       </c>
       <c r="G140" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -3863,22 +3860,22 @@
         <v>43358</v>
       </c>
       <c r="B141" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C141" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D141" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G141" t="s">
+        <v>144</v>
+      </c>
+      <c r="H141" t="s">
         <v>145</v>
       </c>
-      <c r="H141" t="s">
+      <c r="I141" t="s">
         <v>146</v>
-      </c>
-      <c r="I141" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -3984,19 +3981,19 @@
         <v>43679</v>
       </c>
       <c r="B149" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C149" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D149" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E149" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I149" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -4004,16 +4001,16 @@
         <v>43680</v>
       </c>
       <c r="B150" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C150" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D150" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G150" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -4038,16 +4035,16 @@
         <v>30</v>
       </c>
       <c r="E152" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F152">
         <v>245</v>
       </c>
       <c r="G152" t="s">
+        <v>148</v>
+      </c>
+      <c r="H152" t="s">
         <v>149</v>
-      </c>
-      <c r="H152" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -4055,19 +4052,19 @@
         <v>43789</v>
       </c>
       <c r="B153" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E153" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F153">
         <v>380</v>
       </c>
       <c r="G153" t="s">
+        <v>150</v>
+      </c>
+      <c r="H153" t="s">
         <v>151</v>
-      </c>
-      <c r="H153" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -4078,13 +4075,13 @@
         <v>3</v>
       </c>
       <c r="E154" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F154">
         <v>295</v>
       </c>
       <c r="G154" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -4095,16 +4092,16 @@
         <v>23</v>
       </c>
       <c r="E155" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F155">
         <v>189</v>
       </c>
       <c r="G155" t="s">
+        <v>104</v>
+      </c>
+      <c r="H155" t="s">
         <v>105</v>
-      </c>
-      <c r="H155" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -4115,16 +4112,16 @@
         <v>5</v>
       </c>
       <c r="E156" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F156">
         <v>295</v>
       </c>
       <c r="G156" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H156" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -4135,16 +4132,16 @@
         <v>1</v>
       </c>
       <c r="E157" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F157">
         <v>295</v>
       </c>
       <c r="G157" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H157" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -4152,16 +4149,16 @@
         <v>43922</v>
       </c>
       <c r="D158" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E158" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F158">
         <v>145</v>
       </c>
       <c r="G158" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -4178,16 +4175,16 @@
         <v>9</v>
       </c>
       <c r="E159" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F159">
         <v>125</v>
       </c>
       <c r="G159" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I159" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -4198,16 +4195,16 @@
         <v>18</v>
       </c>
       <c r="E160" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F160">
         <v>189</v>
       </c>
       <c r="G160" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H160" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -4218,13 +4215,13 @@
         <v>7</v>
       </c>
       <c r="E161" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F161">
         <v>189</v>
       </c>
       <c r="G161" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -4241,16 +4238,16 @@
         <v>26</v>
       </c>
       <c r="E162" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F162">
         <v>130</v>
       </c>
       <c r="G162" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H162" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -4306,16 +4303,16 @@
         <v>12</v>
       </c>
       <c r="E166" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F166">
         <v>130</v>
       </c>
       <c r="G166" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H166" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -4323,25 +4320,25 @@
         <v>44001</v>
       </c>
       <c r="B167" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C167" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D167" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E167" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F167">
         <v>189</v>
       </c>
       <c r="G167" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H167" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -4358,7 +4355,7 @@
         <v>27</v>
       </c>
       <c r="E168" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -4375,10 +4372,10 @@
         <v>28</v>
       </c>
       <c r="G169" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H169" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -4395,7 +4392,7 @@
         <v>29</v>
       </c>
       <c r="G170" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -4412,16 +4409,16 @@
         <v>30</v>
       </c>
       <c r="E171" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F171">
         <v>245</v>
       </c>
       <c r="G171" t="s">
+        <v>148</v>
+      </c>
+      <c r="H171" t="s">
         <v>149</v>
-      </c>
-      <c r="H171" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -4438,16 +4435,16 @@
         <v>30</v>
       </c>
       <c r="E172" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F172">
         <v>245</v>
       </c>
       <c r="G172" t="s">
+        <v>148</v>
+      </c>
+      <c r="H172" t="s">
         <v>149</v>
-      </c>
-      <c r="H172" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -4458,13 +4455,13 @@
         <v>3</v>
       </c>
       <c r="E173" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F173">
         <v>295</v>
       </c>
       <c r="G173" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -4475,16 +4472,16 @@
         <v>23</v>
       </c>
       <c r="E174" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F174">
         <v>155</v>
       </c>
       <c r="G174" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H174" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -4495,16 +4492,16 @@
         <v>5</v>
       </c>
       <c r="E175" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F175">
         <v>295</v>
       </c>
       <c r="G175" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H175" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -4515,16 +4512,16 @@
         <v>23</v>
       </c>
       <c r="E176" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F176">
         <v>155</v>
       </c>
       <c r="G176" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H176" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -4535,16 +4532,16 @@
         <v>23</v>
       </c>
       <c r="E177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F177">
         <v>155</v>
       </c>
       <c r="G177" t="s">
+        <v>104</v>
+      </c>
+      <c r="H177" t="s">
         <v>105</v>
-      </c>
-      <c r="H177" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -4555,13 +4552,13 @@
         <v>9</v>
       </c>
       <c r="E178" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F178">
         <v>125</v>
       </c>
       <c r="G178" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -4578,16 +4575,16 @@
         <v>18</v>
       </c>
       <c r="E179" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F179">
         <v>155</v>
       </c>
       <c r="G179" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H179" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -4601,16 +4598,16 @@
         <v>12</v>
       </c>
       <c r="E180" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F180">
         <v>245</v>
       </c>
       <c r="G180" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H180" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -4621,13 +4618,13 @@
         <v>7</v>
       </c>
       <c r="E181" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F181">
         <v>130</v>
       </c>
       <c r="G181" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -4638,13 +4635,13 @@
         <v>7</v>
       </c>
       <c r="E182" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F182">
         <v>130</v>
       </c>
       <c r="G182" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -4655,13 +4652,13 @@
         <v>9</v>
       </c>
       <c r="E183" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F183">
         <v>125</v>
       </c>
       <c r="G183" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -4672,16 +4669,16 @@
         <v>18</v>
       </c>
       <c r="E184" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F184">
         <v>245</v>
       </c>
       <c r="G184" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H184" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -4689,16 +4686,16 @@
         <v>44299</v>
       </c>
       <c r="C185" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E185" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F185">
         <v>295</v>
       </c>
       <c r="G185" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
@@ -4715,16 +4712,16 @@
         <v>26</v>
       </c>
       <c r="E186" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F186">
         <v>130</v>
       </c>
       <c r="G186" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H186" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -4769,16 +4766,16 @@
         <v>12</v>
       </c>
       <c r="E189" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F189">
         <v>130</v>
       </c>
       <c r="G189" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H189" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -4795,16 +4792,16 @@
         <v>17</v>
       </c>
       <c r="E190" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F190">
         <v>195</v>
       </c>
       <c r="G190" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H190" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
@@ -4818,16 +4815,16 @@
         <v>9</v>
       </c>
       <c r="E191" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F191">
         <v>195</v>
       </c>
       <c r="G191" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H191" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
@@ -4835,13 +4832,13 @@
         <v>44400</v>
       </c>
       <c r="B192" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C192" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D192" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -4849,16 +4846,16 @@
         <v>44491</v>
       </c>
       <c r="B193" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C193" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D193" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E193" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -4866,19 +4863,19 @@
         <v>44498</v>
       </c>
       <c r="B194" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C194" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D194" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G194" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H194" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -4895,7 +4892,7 @@
         <v>29</v>
       </c>
       <c r="G195" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -4912,16 +4909,16 @@
         <v>30</v>
       </c>
       <c r="E196" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F196">
         <v>245</v>
       </c>
       <c r="G196" t="s">
+        <v>148</v>
+      </c>
+      <c r="H196" t="s">
         <v>149</v>
-      </c>
-      <c r="H196" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -4932,16 +4929,16 @@
         <v>30</v>
       </c>
       <c r="E197" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F197">
         <v>245</v>
       </c>
       <c r="G197" t="s">
+        <v>148</v>
+      </c>
+      <c r="H197" t="s">
         <v>149</v>
-      </c>
-      <c r="H197" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
@@ -4949,22 +4946,22 @@
         <v>44529</v>
       </c>
       <c r="B198" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C198" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D198" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E198" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F198">
         <v>380</v>
       </c>
       <c r="G198" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -4975,13 +4972,13 @@
         <v>3</v>
       </c>
       <c r="E199" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F199">
         <v>295</v>
       </c>
       <c r="G199" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
@@ -4992,16 +4989,16 @@
         <v>23</v>
       </c>
       <c r="E200" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F200">
         <v>155</v>
       </c>
       <c r="G200" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H200" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
@@ -5012,16 +5009,16 @@
         <v>5</v>
       </c>
       <c r="E201" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F201">
         <v>295</v>
       </c>
       <c r="G201" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H201" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
@@ -5032,16 +5029,16 @@
         <v>23</v>
       </c>
       <c r="E202" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F202">
         <v>195</v>
       </c>
       <c r="G202" t="s">
+        <v>104</v>
+      </c>
+      <c r="H202" t="s">
         <v>105</v>
-      </c>
-      <c r="H202" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
@@ -5052,16 +5049,16 @@
         <v>12</v>
       </c>
       <c r="E203" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F203">
         <v>130</v>
       </c>
       <c r="G203" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H203" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
@@ -5075,16 +5072,16 @@
         <v>30</v>
       </c>
       <c r="E204" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F204">
         <v>245</v>
       </c>
       <c r="G204" t="s">
+        <v>148</v>
+      </c>
+      <c r="H204" t="s">
         <v>149</v>
-      </c>
-      <c r="H204" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
@@ -5095,13 +5092,13 @@
         <v>1</v>
       </c>
       <c r="E205" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F205">
         <v>245</v>
       </c>
       <c r="G205" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
@@ -5118,16 +5115,16 @@
         <v>18</v>
       </c>
       <c r="E206" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F206">
         <v>245</v>
       </c>
       <c r="G206" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H206" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
@@ -5144,13 +5141,13 @@
         <v>9</v>
       </c>
       <c r="E207" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F207">
         <v>125</v>
       </c>
       <c r="G207" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
@@ -5167,13 +5164,13 @@
         <v>7</v>
       </c>
       <c r="E208" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F208">
         <v>130</v>
       </c>
       <c r="G208" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
@@ -5181,25 +5178,25 @@
         <v>44680</v>
       </c>
       <c r="B209" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C209" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D209" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E209" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F209">
         <v>130</v>
       </c>
       <c r="G209" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H209" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
@@ -5230,16 +5227,16 @@
         <v>12</v>
       </c>
       <c r="E211" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F211">
         <v>295</v>
       </c>
       <c r="G211" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H211" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -5256,16 +5253,16 @@
         <v>17</v>
       </c>
       <c r="E212" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F212">
         <v>125</v>
       </c>
       <c r="G212" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H212" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -5282,16 +5279,16 @@
         <v>9</v>
       </c>
       <c r="E213" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F213">
         <v>195</v>
       </c>
       <c r="G213" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H213" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -5299,16 +5296,16 @@
         <v>44858</v>
       </c>
       <c r="B214" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C214" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D214" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E214" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
@@ -5316,19 +5313,19 @@
         <v>44867</v>
       </c>
       <c r="B215" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C215" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D215" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G215" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H215" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
@@ -5336,16 +5333,16 @@
         <v>44867</v>
       </c>
       <c r="B216" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C216" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D216" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G216" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -5356,13 +5353,13 @@
         <v>3</v>
       </c>
       <c r="E217" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F217">
         <v>295</v>
       </c>
       <c r="G217" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -5379,16 +5376,16 @@
         <v>30</v>
       </c>
       <c r="E218" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F218">
         <v>245</v>
       </c>
       <c r="G218" t="s">
+        <v>148</v>
+      </c>
+      <c r="H218" t="s">
         <v>149</v>
-      </c>
-      <c r="H218" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -5399,16 +5396,16 @@
         <v>23</v>
       </c>
       <c r="E219" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F219">
         <v>155</v>
       </c>
       <c r="G219" t="s">
+        <v>104</v>
+      </c>
+      <c r="H219" t="s">
         <v>105</v>
-      </c>
-      <c r="H219" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -5419,16 +5416,16 @@
         <v>23</v>
       </c>
       <c r="E220" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F220">
         <v>155</v>
       </c>
       <c r="G220" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H220" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -5439,16 +5436,16 @@
         <v>5</v>
       </c>
       <c r="E221" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F221">
         <v>295</v>
       </c>
       <c r="G221" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H221" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -5459,16 +5456,16 @@
         <v>23</v>
       </c>
       <c r="E222" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F222">
         <v>195</v>
       </c>
       <c r="G222" t="s">
+        <v>104</v>
+      </c>
+      <c r="H222" t="s">
         <v>105</v>
-      </c>
-      <c r="H222" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -5479,22 +5476,22 @@
         <v>18</v>
       </c>
       <c r="C223" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D223" t="s">
         <v>18</v>
       </c>
       <c r="E223" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F223">
         <v>245</v>
       </c>
       <c r="G223" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H223" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -5508,13 +5505,13 @@
         <v>9</v>
       </c>
       <c r="E224" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F224">
         <v>125</v>
       </c>
       <c r="G224" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
@@ -5528,13 +5525,13 @@
         <v>7</v>
       </c>
       <c r="E225" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F225">
         <v>130</v>
       </c>
       <c r="G225" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
@@ -5542,16 +5539,16 @@
         <v>45030</v>
       </c>
       <c r="C226" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E226" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F226">
         <v>295</v>
       </c>
       <c r="G226" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -5568,16 +5565,16 @@
         <v>9</v>
       </c>
       <c r="E227" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F227">
         <v>195</v>
       </c>
       <c r="G227" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H227" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -5594,19 +5591,19 @@
         <v>19</v>
       </c>
       <c r="E228" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F228">
         <v>195</v>
       </c>
       <c r="G228" t="s">
+        <v>164</v>
+      </c>
+      <c r="H228" t="s">
+        <v>74</v>
+      </c>
+      <c r="I228" t="s">
         <v>165</v>
-      </c>
-      <c r="H228" t="s">
-        <v>75</v>
-      </c>
-      <c r="I228" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
@@ -5637,19 +5634,19 @@
         <v>9</v>
       </c>
       <c r="E230" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F230">
         <v>245</v>
       </c>
       <c r="G230" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H230" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I230" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
@@ -5666,16 +5663,16 @@
         <v>12</v>
       </c>
       <c r="E231" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F231">
         <v>155</v>
       </c>
       <c r="G231" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H231" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
@@ -5692,16 +5689,16 @@
         <v>35</v>
       </c>
       <c r="E232" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F232">
         <v>125</v>
       </c>
       <c r="G232" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H232" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -5718,7 +5715,7 @@
         <v>21</v>
       </c>
       <c r="E233" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
@@ -5735,16 +5732,16 @@
         <v>30</v>
       </c>
       <c r="E234" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F234">
         <v>295</v>
       </c>
       <c r="G234" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H234" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
@@ -5761,13 +5758,13 @@
         <v>9</v>
       </c>
       <c r="E235" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F235">
         <v>125</v>
       </c>
       <c r="G235" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
@@ -5784,16 +5781,16 @@
         <v>18</v>
       </c>
       <c r="E236" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F236">
         <v>245</v>
       </c>
       <c r="G236" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H236" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -5810,13 +5807,13 @@
         <v>7</v>
       </c>
       <c r="E237" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F237">
         <v>125</v>
       </c>
       <c r="G237" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
@@ -5824,19 +5821,19 @@
         <v>45182</v>
       </c>
       <c r="B238" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C238" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D238" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G238" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I238" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
@@ -5844,13 +5841,13 @@
         <v>45616</v>
       </c>
       <c r="B239" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E239" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G239" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
@@ -5864,16 +5861,16 @@
         <v>30</v>
       </c>
       <c r="E240" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F240">
         <v>245</v>
       </c>
       <c r="G240" t="s">
+        <v>148</v>
+      </c>
+      <c r="H240" t="s">
         <v>149</v>
-      </c>
-      <c r="H240" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
@@ -5884,13 +5881,13 @@
         <v>3</v>
       </c>
       <c r="E241" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F241">
         <v>295</v>
       </c>
       <c r="G241" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -5901,16 +5898,16 @@
         <v>23</v>
       </c>
       <c r="E242" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F242">
         <v>195</v>
       </c>
       <c r="G242" t="s">
+        <v>104</v>
+      </c>
+      <c r="H242" t="s">
         <v>105</v>
-      </c>
-      <c r="H242" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
@@ -5921,16 +5918,16 @@
         <v>23</v>
       </c>
       <c r="E243" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F243">
         <v>195</v>
       </c>
       <c r="G243" t="s">
+        <v>104</v>
+      </c>
+      <c r="H243" t="s">
         <v>105</v>
-      </c>
-      <c r="H243" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
@@ -5941,13 +5938,13 @@
         <v>5</v>
       </c>
       <c r="E244" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F244">
         <v>295</v>
       </c>
       <c r="G244" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
@@ -5958,16 +5955,16 @@
         <v>23</v>
       </c>
       <c r="E245" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F245">
         <v>155</v>
       </c>
       <c r="G245" t="s">
+        <v>104</v>
+      </c>
+      <c r="H245" t="s">
         <v>105</v>
-      </c>
-      <c r="H245" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
@@ -5978,13 +5975,13 @@
         <v>18</v>
       </c>
       <c r="E246" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F246">
         <v>245</v>
       </c>
       <c r="G246" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
@@ -5995,13 +5992,13 @@
         <v>7</v>
       </c>
       <c r="E247" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F247">
         <v>130</v>
       </c>
       <c r="G247" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
@@ -6018,13 +6015,13 @@
         <v>7</v>
       </c>
       <c r="E248" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F248">
         <v>130</v>
       </c>
       <c r="G248" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
@@ -6038,10 +6035,10 @@
         <v>9</v>
       </c>
       <c r="G249" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I249" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
@@ -6055,13 +6052,13 @@
         <v>17</v>
       </c>
       <c r="E250" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F250">
         <v>125</v>
       </c>
       <c r="G250" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I250" s="3"/>
     </row>
@@ -6073,16 +6070,16 @@
         <v>9</v>
       </c>
       <c r="E251" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F251">
         <v>195</v>
       </c>
       <c r="G251" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I251" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
@@ -6090,16 +6087,16 @@
         <v>45757</v>
       </c>
       <c r="C252" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E252" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F252">
         <v>295</v>
       </c>
       <c r="G252" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
@@ -6116,13 +6113,13 @@
         <v>18</v>
       </c>
       <c r="E253" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G253" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I253" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
@@ -6139,13 +6136,13 @@
         <v>7</v>
       </c>
       <c r="E254" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F254">
         <v>130</v>
       </c>
       <c r="G254" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
@@ -6153,25 +6150,25 @@
         <v>45771</v>
       </c>
       <c r="B255" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C255" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D255" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E255" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F255">
         <v>130</v>
       </c>
       <c r="G255" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H255" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
@@ -6188,13 +6185,13 @@
         <v>9</v>
       </c>
       <c r="E256" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G256" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I256" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="I256" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
@@ -6211,13 +6208,13 @@
         <v>17</v>
       </c>
       <c r="E257" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F257">
         <v>125</v>
       </c>
       <c r="G257" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
@@ -6234,13 +6231,13 @@
         <v>12</v>
       </c>
       <c r="E258" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G258" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H258" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
@@ -6248,22 +6245,22 @@
         <v>45832</v>
       </c>
       <c r="B259" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C259" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D259" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E259" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F259">
         <v>156</v>
       </c>
       <c r="G259" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>